<commit_message>
Image Status and Download
</commit_message>
<xml_diff>
--- a/UMS_Test/TestData/Student/Image/ImageStatus/ImageStatusData.xlsx
+++ b/UMS_Test/TestData/Student/Image/ImageStatus/ImageStatusData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OPL\source\repos\UMS_Test\UMS_Test\TestData\Student\Image\ImageStatus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A10F324-6D45-45F4-89AF-A757241FA6CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3A486C8-96FC-470B-A723-BC8EFB7442D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="53">
   <si>
     <t>Batch</t>
   </si>
@@ -84,9 +84,6 @@
     <t xml:space="preserve"> Farmgate (MT) Udvash</t>
   </si>
   <si>
-    <t>Roll No., Nick Name, Full Name</t>
-  </si>
-  <si>
     <t>udvash</t>
   </si>
   <si>
@@ -166,6 +163,27 @@
   </si>
   <si>
     <t>Combo</t>
+  </si>
+  <si>
+    <t>roll , image, Mobile Number</t>
+  </si>
+  <si>
+    <t>Registration No, Full Name, Mobile Number(Student)</t>
+  </si>
+  <si>
+    <t>Roll No., Nick Name, Full Name, Mobile Number(Father)</t>
+  </si>
+  <si>
+    <t>Akash</t>
+  </si>
+  <si>
+    <t>Mahi</t>
+  </si>
+  <si>
+    <t>01781770073</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select All </t>
   </si>
 </sst>
 </file>
@@ -201,9 +219,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -488,7 +509,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
@@ -505,15 +526,15 @@
     <col min="9" max="9" width="25.42578125" style="1" customWidth="1"/>
     <col min="10" max="10" width="25.85546875" style="1" customWidth="1"/>
     <col min="11" max="11" width="16.28515625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="13.140625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="11.140625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.5703125" style="1" customWidth="1"/>
     <col min="14" max="14" width="11" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15" style="1" customWidth="1"/>
+    <col min="15" max="15" width="18.42578125" style="2" customWidth="1"/>
     <col min="16" max="16" width="14.140625" style="1" customWidth="1"/>
     <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -556,7 +577,7 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
@@ -565,19 +586,19 @@
     </row>
     <row r="2" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>20</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="1">
         <v>2024</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>17</v>
@@ -586,19 +607,19 @@
         <v>18</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>47</v>
       </c>
       <c r="P2" s="1" t="s">
         <v>16</v>
@@ -606,40 +627,40 @@
     </row>
     <row r="3" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" s="1">
         <v>2024</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>46</v>
       </c>
       <c r="P3" s="1" t="s">
         <v>16</v>
@@ -647,40 +668,46 @@
     </row>
     <row r="4" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="1">
         <v>2024</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>19</v>
+        <v>48</v>
+      </c>
+      <c r="M4" s="1">
+        <v>10216600311</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>16</v>
@@ -688,40 +715,49 @@
     </row>
     <row r="5" spans="1:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1">
         <v>2024</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I5" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>52</v>
+      </c>
+      <c r="M5" s="1">
+        <v>3309937</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="O5" s="2" t="s">
+        <v>51</v>
       </c>
       <c r="P5" s="1" t="s">
         <v>16</v>

</xml_diff>